<commit_message>
HierarchialReportModel and updated tests and template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91C4FE7-F30D-4EA7-8AE4-D487BF7106F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D6488C-87C5-4E99-8A92-0D10519BDE9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EFA HNS Summary Report" sheetId="3" r:id="rId1"/>
@@ -163,66 +163,6 @@
     <t>&amp;=HNSSummary.Year</t>
   </si>
   <si>
-    <t>&amp;=HNSSummary.TotalDirectFunded1416_WithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.TotalDirectFunded1416_WithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.TotalDirectFunded1416_HNSWithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.TotalDirectFunded1416_HNSWithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.TotalDirectFunded1416_EHCPWithoutHNS</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1619IncludingHNS_WithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1619IncludingHNS_WithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1619IncludingHNS_HNSWithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1619IncludingHNS_HNSWithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1619IncludingHNS_EHCPWithoutHNS</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1924WithEHCP_WithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1924WithEHCP_WithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1924WithEHCP_HNSWithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1924WithEHCP_HNSWithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total1924WithEHCP_EHCPWithoutHNS</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total19PlusWithoutEHCP_WithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total19PlusWithoutEHCP_WithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total19PlusWithoutEHCP_HNSWithoutEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total19PlusWithoutEHCP_HNSWithEHCP</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.Total19PlusWithoutEHCP_EHCPWithoutHNS</t>
-  </si>
-  <si>
     <t>&amp;=HNSSummary.LarsData</t>
   </si>
   <si>
@@ -254,6 +194,66 @@
   </si>
   <si>
     <t>&amp;=HNSSummary.ReportGeneratedAt</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.WithEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.WithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.HNSWithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.EHCPWithHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.EHCPWithoutHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.WithEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.WithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.HNSWithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.EHCPWithoutHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.EHCPWithHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.WithEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.WithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.HNSWithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.EHCPWithHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.EHCPWithoutHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.WithEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.WithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.HNSWithoutEHCP</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.EHCPWithHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.EHCPWithoutHNS</t>
   </si>
 </sst>
 </file>
@@ -675,6 +675,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
       <protection locked="0"/>
@@ -698,6 +701,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -722,9 +728,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -765,9 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A107" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1779,10 +1779,10 @@
       <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
@@ -1792,10 +1792,10 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="31" t="s">
         <v>3</v>
       </c>
@@ -1826,97 +1826,97 @@
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="58"/>
       <c r="G11" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="51" t="s">
+      <c r="C12" s="60"/>
+      <c r="D12" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="67" t="s">
-        <v>45</v>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="42" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="51" t="s">
+      <c r="A13" s="67"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="18" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="66"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="48" t="s">
+      <c r="A14" s="67"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="18" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="48" t="s">
+      <c r="A15" s="67"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="50"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="18" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="66"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="48" t="s">
+      <c r="A16" s="67"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="18" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="51" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="18">
         <f>SUM(G12:G16)</f>
         <v>0</v>
@@ -1939,11 +1939,11 @@
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="23" t="s">
         <v>4</v>
       </c>
@@ -1951,93 +1951,93 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="51" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="67" t="s">
-        <v>50</v>
+      <c r="E20" s="54"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="42" t="s">
+        <v>56</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="66"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="51" t="s">
+      <c r="A21" s="67"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="19" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="66"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="48" t="s">
+      <c r="A22" s="67"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="49"/>
-      <c r="F22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="52"/>
       <c r="G22" s="19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="66"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="48" t="s">
+      <c r="A23" s="67"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="52"/>
       <c r="G23" s="19" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="66"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="48" t="s">
+      <c r="A24" s="67"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="52"/>
       <c r="G24" s="19" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="66"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="51" t="s">
+      <c r="A25" s="67"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
       <c r="G25" s="19">
         <f>SUM(G20:G24)</f>
         <v>0</v>
@@ -2060,11 +2060,11 @@
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
       <c r="G27" s="23" t="s">
         <v>4</v>
       </c>
@@ -2072,93 +2072,93 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="51" t="s">
+      <c r="C28" s="60"/>
+      <c r="D28" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="52"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="67" t="s">
-        <v>55</v>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="42" t="s">
+        <v>61</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="66"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="51" t="s">
+      <c r="A29" s="67"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
       <c r="G29" s="20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="66"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="48" t="s">
+      <c r="A30" s="67"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="52"/>
       <c r="G30" s="20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="66"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="48" t="s">
+      <c r="A31" s="67"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="52"/>
       <c r="G31" s="20" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="66"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="48" t="s">
+      <c r="A32" s="67"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="20" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="66"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="51" t="s">
+      <c r="A33" s="67"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="52"/>
-      <c r="F33" s="53"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55"/>
       <c r="G33" s="20">
         <f>SUM(G28:G32)</f>
         <v>0</v>
@@ -2181,11 +2181,11 @@
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="56"/>
-      <c r="F35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
       <c r="G35" s="23" t="s">
         <v>4</v>
       </c>
@@ -2193,93 +2193,93 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="51" t="s">
+      <c r="C36" s="60"/>
+      <c r="D36" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="52"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="67" t="s">
-        <v>60</v>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="42" t="s">
+        <v>66</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="66"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="51" t="s">
+      <c r="A37" s="67"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="53"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="55"/>
       <c r="G37" s="21" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="66"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="48" t="s">
+      <c r="A38" s="67"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="52"/>
       <c r="G38" s="21" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="66"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="48" t="s">
+      <c r="A39" s="67"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="52"/>
       <c r="G39" s="21" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="66"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="48" t="s">
+      <c r="A40" s="67"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="52"/>
       <c r="G40" s="21" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="66"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="51" t="s">
+      <c r="A41" s="67"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="52"/>
-      <c r="F41" s="53"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
       <c r="G41" s="21">
         <f>SUM(G36:G40)</f>
         <v>0</v>
@@ -2302,11 +2302,11 @@
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="51" t="s">
+      <c r="D43" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="52"/>
-      <c r="F43" s="53"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
       <c r="G43" s="21">
         <f>SUM(G17,G25,G33,G41)</f>
         <v>0</v>
@@ -2316,11 +2316,11 @@
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="46"/>
-      <c r="F44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="48"/>
       <c r="G44" s="21">
         <f>SUM(G39,G38,G31,G30,G23,G22,G15,G14)</f>
         <v>0</v>
@@ -2372,82 +2372,82 @@
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="54" t="s">
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
     </row>
     <row r="51" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="42" t="s">
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
     </row>
     <row r="52" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="42" t="s">
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
     </row>
     <row r="53" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="42" t="s">
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
     </row>
     <row r="54" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="42" t="s">
+      <c r="B54" s="45"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
     </row>
     <row r="55" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="42" t="s">
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
     </row>
     <row r="56" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
@@ -3046,51 +3046,51 @@
     </row>
     <row r="121" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="40" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B121" s="40"/>
-      <c r="C121" s="41" t="s">
-        <v>74</v>
+      <c r="C121" s="40" t="s">
+        <v>54</v>
       </c>
       <c r="D121" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F121" s="43"/>
+      <c r="E121" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F121" s="44"/>
       <c r="G121" s="36"/>
     </row>
     <row r="122" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A122" s="41" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B122" s="41"/>
       <c r="C122" s="41" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D122" s="33" t="s">
         <v>14</v>
       </c>
       <c r="E122" s="37" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F122" s="37"/>
       <c r="G122" s="37"/>
     </row>
     <row r="123" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A123" s="41" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B123" s="41"/>
       <c r="C123" s="41" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D123" s="33" t="s">
         <v>15</v>
       </c>
       <c r="E123" s="37" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F123" s="37"/>
       <c r="G123" s="37"/>
@@ -3103,14 +3103,14 @@
         <v>16</v>
       </c>
       <c r="E124" s="37" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F124" s="37"/>
       <c r="G124" s="37"/>
     </row>
     <row r="125" spans="1:17" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A125" s="41" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B125" s="37"/>
       <c r="C125" s="37"/>

</xml_diff>

<commit_message>
Bug fixes - 87013,86919,87120,86913,86916
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D6488C-87C5-4E99-8A92-0D10519BDE9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FF9BC2-3094-42A0-8F9E-03A4C8613343}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EFA HNS Summary Report" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>Provider :</t>
   </si>
@@ -187,12 +187,6 @@
     <t>&amp;=HNSSummary.ApplicationVersion</t>
   </si>
   <si>
-    <t>Component Set Version:</t>
-  </si>
-  <si>
-    <t>&amp;=HNSSummary.ComponentSetVersion</t>
-  </si>
-  <si>
     <t>&amp;=HNSSummary.ReportGeneratedAt</t>
   </si>
   <si>
@@ -254,6 +248,18 @@
   </si>
   <si>
     <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.EHCPWithoutHNS</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.DirectFunded1416StudentsTotal.TotalFundineStudents</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.IncludingHNS1619StudentsTotal.TotalFundineStudents</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.EHCP1924StudentsTotal.TotalFundineStudents</t>
+  </si>
+  <si>
+    <t>&amp;=HNSSummary.Continuing19PlusExcludingEHCPStudentsTotal.TotalFundineStudents</t>
   </si>
 </sst>
 </file>
@@ -675,8 +681,74 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -685,10 +757,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -704,70 +772,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1687,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A107" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1779,10 +1785,10 @@
       <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="65"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
@@ -1792,10 +1798,10 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="65"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="31" t="s">
         <v>3</v>
       </c>
@@ -1826,100 +1832,99 @@
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="57"/>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="53" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="42" t="s">
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="45"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="45"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="67"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="18" t="s">
+    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="45"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="18" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="67"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="67"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="67"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="50" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="52"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="67"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="53" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="18">
-        <f>SUM(G12:G16)</f>
-        <v>0</v>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1939,11 +1944,11 @@
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="54"/>
       <c r="G19" s="23" t="s">
         <v>4</v>
       </c>
@@ -1951,96 +1956,95 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="53" t="s">
+      <c r="C20" s="47"/>
+      <c r="D20" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="42" t="s">
-        <v>56</v>
+      <c r="E20" s="56"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="67" t="s">
+        <v>54</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="67"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="53" t="s">
+      <c r="A21" s="45"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
       <c r="G21" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="67"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="50" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="67"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="50" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="52"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="67"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="50" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
       <c r="G24" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="67"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="53" t="s">
+      <c r="A25" s="45"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="19">
-        <f>SUM(G20:G24)</f>
-        <v>0</v>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2060,11 +2064,11 @@
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="56" t="s">
+      <c r="D27" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="23" t="s">
         <v>4</v>
       </c>
@@ -2072,96 +2076,95 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="53" t="s">
+      <c r="C28" s="47"/>
+      <c r="D28" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="54"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="42" t="s">
-        <v>61</v>
+      <c r="E28" s="56"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="67" t="s">
+        <v>59</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="53" t="s">
+      <c r="A29" s="45"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="54"/>
-      <c r="F29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="57"/>
       <c r="G29" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="50" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="51"/>
-      <c r="F30" s="52"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="50" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="51"/>
-      <c r="F31" s="52"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="67"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="50" t="s">
+      <c r="A32" s="45"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="53" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="20">
-        <f>SUM(G28:G32)</f>
-        <v>0</v>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2181,11 +2184,11 @@
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="54"/>
       <c r="G35" s="23" t="s">
         <v>4</v>
       </c>
@@ -2193,96 +2196,95 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="67" t="s">
+      <c r="A36" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="60"/>
-      <c r="D36" s="53" t="s">
+      <c r="C36" s="47"/>
+      <c r="D36" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="42" t="s">
-        <v>66</v>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="67" t="s">
+        <v>64</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="67"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="53" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="55"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="57"/>
       <c r="G37" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="67"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="50" t="s">
+      <c r="A38" s="45"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="F38" s="52"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="67"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="50" t="s">
+      <c r="A39" s="45"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="52"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="60"/>
       <c r="G39" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="67"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="50" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="52"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="60"/>
       <c r="G40" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="67"/>
-      <c r="B41" s="63"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="53" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="54"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="21">
-        <f>SUM(G36:G40)</f>
-        <v>0</v>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="21" t="s">
+        <v>77</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2302,11 +2304,11 @@
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="53" t="s">
+      <c r="D43" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="54"/>
-      <c r="F43" s="55"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="57"/>
       <c r="G43" s="21">
         <f>SUM(G17,G25,G33,G41)</f>
         <v>0</v>
@@ -2316,11 +2318,11 @@
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="46" t="s">
+      <c r="D44" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="48"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="65"/>
       <c r="G44" s="21">
         <f>SUM(G39,G38,G31,G30,G23,G22,G15,G14)</f>
         <v>0</v>
@@ -2372,82 +2374,82 @@
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="66"/>
-      <c r="C50" s="66"/>
-      <c r="D50" s="49" t="s">
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="66"/>
     </row>
     <row r="51" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="43" t="s">
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
     </row>
     <row r="52" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="43" t="s">
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
     </row>
     <row r="53" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="43" t="s">
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
     </row>
     <row r="54" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="43" t="s">
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
     </row>
     <row r="55" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="43" t="s">
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
     </row>
     <row r="56" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
@@ -3046,28 +3048,28 @@
     </row>
     <row r="121" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B121" s="40"/>
       <c r="C121" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D121" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="44" t="s">
+      <c r="E121" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="F121" s="44"/>
+      <c r="F121" s="62"/>
       <c r="G121" s="36"/>
     </row>
     <row r="122" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A122" s="41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B122" s="41"/>
       <c r="C122" s="41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D122" s="33" t="s">
         <v>14</v>
@@ -3079,13 +3081,6 @@
       <c r="G122" s="37"/>
     </row>
     <row r="123" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A123" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B123" s="41"/>
-      <c r="C123" s="41" t="s">
-        <v>50</v>
-      </c>
       <c r="D123" s="33" t="s">
         <v>15</v>
       </c>
@@ -3110,7 +3105,7 @@
     </row>
     <row r="125" spans="1:17" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A125" s="41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B125" s="37"/>
       <c r="C125" s="37"/>
@@ -3131,6 +3126,47 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B20:C25"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="B12:C17"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A51:C51"/>
@@ -3143,47 +3179,6 @@
     <mergeCell ref="B36:C41"/>
     <mergeCell ref="B28:C33"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="B12:C17"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="A55:C55"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="70" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3339,12 +3334,7 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3363,7 +3353,12 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3384,9 +3379,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3407,9 +3402,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed footnote 5 from HNS excel template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/HNSSummaryReportTemplate.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CADC6B8-8348-4E1A-873E-D7756013ABCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-405" yWindow="-16320" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -337,7 +336,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -755,6 +754,90 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -767,29 +850,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -802,79 +862,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Currency 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -981,7 +980,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC59D13E-2AB6-4C1A-A925-77D12CAD0C2B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC59D13E-2AB6-4C1A-A925-77D12CAD0C2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1425,39 +1424,6 @@
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>5)  All factors displayed in this report and used in funding calculations are those used in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>your 2020 to 2021 allocation</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -1485,7 +1451,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9267AB-7DB8-4D57-ABF7-D457205DB273}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6A9267AB-7DB8-4D57-ABF7-D457205DB273}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1928,39 +1894,6 @@
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>5)  All factors displayed in this report and used in funding calculations are those used in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>your 2020 to 2021 allocation</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2045,23 +1978,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2097,23 +2013,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2289,29 +2188,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5859375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.87890625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.29296875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="7" max="7" width="21.28515625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>29</v>
       </c>
@@ -2325,7 +2222,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2334,7 +2231,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
@@ -2347,7 +2244,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
@@ -2360,7 +2257,7 @@
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
@@ -2377,7 +2274,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="25"/>
@@ -2386,128 +2283,128 @@
       <c r="F6" s="26"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:9" ht="12.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="58" t="s">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="63"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="63" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="64"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="67" t="s">
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="50" t="s">
+    <row r="10" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="50"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="42" t="s">
+    <row r="11" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="37" t="s">
+    <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="37" t="s">
+    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="15" t="s">
         <v>56</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="37" t="s">
+    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="50"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="42" t="s">
+    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="46"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="15" t="s">
         <v>58</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2518,116 +2415,116 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="50" t="s">
+    <row r="18" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="42" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="36" t="s">
         <v>59</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="50"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="42" t="s">
+    <row r="19" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="46"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
       <c r="G19" s="16" t="s">
         <v>60</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="37" t="s">
+    <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="46"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="16" t="s">
         <v>61</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="50"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="37" t="s">
+    <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="46"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="16" t="s">
         <v>62</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="50"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="37" t="s">
+    <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="46"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
       <c r="G22" s="16" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="50"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="42" t="s">
+    <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="16" t="s">
         <v>64</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2638,116 +2535,116 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
       <c r="G25" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="50" t="s">
+    <row r="26" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="42" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="36" t="s">
         <v>65</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="50"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="42" t="s">
+    <row r="27" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="46"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="17" t="s">
         <v>66</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="50"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="37" t="s">
+    <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="46"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
       <c r="G28" s="17" t="s">
         <v>67</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="50"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="37" t="s">
+    <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="46"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="17" t="s">
         <v>68</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="50"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="37" t="s">
+    <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="64"/>
       <c r="G30" s="17" t="s">
         <v>69</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="50"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="42" t="s">
+    <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="46"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="17" t="s">
         <v>70</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -2758,116 +2655,116 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="47"/>
-      <c r="F33" s="48"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
       <c r="G33" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="50" t="s">
+    <row r="34" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="42" t="s">
+      <c r="C34" s="48"/>
+      <c r="D34" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="36" t="s">
         <v>71</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="50"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="42" t="s">
+    <row r="35" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="46"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="18" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="50"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="37" t="s">
+    <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="46"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="18" t="s">
         <v>73</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="50"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="37" t="s">
+    <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="46"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="18" t="s">
         <v>74</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="50"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="37" t="s">
+    <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="46"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="64"/>
       <c r="G38" s="18" t="s">
         <v>75</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="50"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="42" t="s">
+    <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="46"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="43"/>
-      <c r="F39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="45"/>
       <c r="G39" s="18" t="s">
         <v>76</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
@@ -2878,35 +2775,35 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="18">
         <f>SUM(G15,G23,G31,G39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="60" t="s">
+      <c r="D42" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="61"/>
-      <c r="F42" s="62"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="59"/>
       <c r="G42" s="18">
         <f>SUM(G37,G36,G29,G28,G21,G20,G13,G12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2915,7 +2812,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2924,85 +2821,85 @@
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="49" t="s">
+    <row r="45" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="45" t="s">
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="41" t="s">
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="40" t="s">
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-    </row>
-    <row r="47" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="41" t="s">
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+    </row>
+    <row r="47" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="40" t="s">
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-    </row>
-    <row r="48" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="41" t="s">
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="40" t="s">
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-    </row>
-    <row r="49" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="41" t="s">
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+    </row>
+    <row r="49" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="40" t="s">
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-    </row>
-    <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="41" t="s">
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+    </row>
+    <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="40" t="s">
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-    </row>
-    <row r="51" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+    </row>
+    <row r="51" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -3011,7 +2908,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -3020,7 +2917,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:17" s="33" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:17" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
       <c r="B53" s="35"/>
       <c r="C53" s="35"/>
@@ -3039,7 +2936,7 @@
       <c r="P53" s="31"/>
       <c r="Q53" s="31"/>
     </row>
-    <row r="54" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -3048,7 +2945,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -3057,7 +2954,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -3066,7 +2963,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -3075,7 +2972,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -3084,7 +2981,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -3093,7 +2990,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -3102,7 +2999,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -3111,7 +3008,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -3120,7 +3017,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -3129,7 +3026,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="34" t="s">
         <v>48</v>
       </c>
@@ -3140,13 +3037,13 @@
       <c r="D64" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E64" s="57" t="s">
+      <c r="E64" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="57"/>
+      <c r="F64" s="53"/>
       <c r="G64" s="34"/>
     </row>
-    <row r="65" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="35" t="s">
         <v>46</v>
       </c>
@@ -3163,7 +3060,7 @@
       <c r="F65" s="35"/>
       <c r="G65" s="35"/>
     </row>
-    <row r="66" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="D66" s="29" t="s">
         <v>13</v>
       </c>
@@ -3173,7 +3070,7 @@
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
     </row>
-    <row r="67" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="6"/>
@@ -3186,7 +3083,7 @@
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
     </row>
-    <row r="68" spans="1:17" s="33" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:17" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="35" t="s">
         <v>50</v>
       </c>
@@ -3209,11 +3106,37 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:C15"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="E64:F64"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="A34:A39"/>
@@ -3230,38 +3153,12 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:C15"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A47:C47"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
@@ -3273,29 +3170,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B98AC-D7B7-4658-BBE3-B6DC5DFA4520}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5859375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.87890625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.29296875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="7" max="7" width="21.28515625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>29</v>
       </c>
@@ -3309,7 +3204,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3318,7 +3213,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3226,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
@@ -3344,7 +3239,7 @@
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
@@ -3361,7 +3256,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="25"/>
@@ -3370,128 +3265,128 @@
       <c r="F6" s="26"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:9" ht="12.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="58" t="s">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="50" t="s">
+    <row r="10" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="50"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="42" t="s">
+    <row r="11" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="37" t="s">
+    <row r="12" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="37" t="s">
+    <row r="13" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="15" t="s">
         <v>80</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="37" t="s">
+    <row r="14" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="15" t="s">
         <v>81</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="50"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="42" t="s">
+    <row r="15" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="46"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="15" t="s">
         <v>82</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3502,116 +3397,116 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="50" t="s">
+    <row r="18" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="42" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="36" t="s">
         <v>83</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="50"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="42" t="s">
+    <row r="19" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="46"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
       <c r="G19" s="16" t="s">
         <v>84</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="37" t="s">
+    <row r="20" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="46"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="16" t="s">
         <v>85</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="50"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="37" t="s">
+    <row r="21" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="46"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="16" t="s">
         <v>86</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="50"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="37" t="s">
+    <row r="22" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="46"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
       <c r="G22" s="16" t="s">
         <v>87</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="50"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="42" t="s">
+    <row r="23" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="16" t="s">
         <v>88</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3622,116 +3517,116 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
       <c r="G25" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="50" t="s">
+    <row r="26" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="42" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="36" t="s">
         <v>89</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="50"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="42" t="s">
+    <row r="27" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="46"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="17" t="s">
         <v>90</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="50"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="37" t="s">
+    <row r="28" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="46"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
       <c r="G28" s="17" t="s">
         <v>91</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="50"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="37" t="s">
+    <row r="29" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="46"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="17" t="s">
         <v>92</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="50"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="37" t="s">
+    <row r="30" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="64"/>
       <c r="G30" s="17" t="s">
         <v>93</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="50"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="42" t="s">
+    <row r="31" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="46"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="17" t="s">
         <v>94</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -3742,116 +3637,116 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="47"/>
-      <c r="F33" s="48"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
       <c r="G33" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="50" t="s">
+    <row r="34" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="42" t="s">
+      <c r="C34" s="48"/>
+      <c r="D34" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="36" t="s">
         <v>95</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="50"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="42" t="s">
+    <row r="35" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="46"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="18" t="s">
         <v>96</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="50"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="37" t="s">
+    <row r="36" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="46"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="18" t="s">
         <v>97</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="50"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="37" t="s">
+    <row r="37" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="46"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="18" t="s">
         <v>98</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="50"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="37" t="s">
+    <row r="38" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="46"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="64"/>
       <c r="G38" s="18" t="s">
         <v>99</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="50"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="42" t="s">
+    <row r="39" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="46"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="43"/>
-      <c r="F39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="45"/>
       <c r="G39" s="18" t="s">
         <v>100</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
@@ -3862,35 +3757,35 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="18">
         <f>SUM(G15,G23,G31,G39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="60" t="s">
+      <c r="D42" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="61"/>
-      <c r="F42" s="62"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="59"/>
       <c r="G42" s="18">
         <f>SUM(G37,G36,G29,G28,G21,G20,G13,G12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -3899,7 +3794,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -3908,85 +3803,85 @@
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="49" t="s">
+    <row r="45" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="45" t="s">
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="41" t="s">
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="40" t="s">
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-    </row>
-    <row r="47" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="41" t="s">
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+    </row>
+    <row r="47" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="40" t="s">
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-    </row>
-    <row r="48" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="41" t="s">
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="40" t="s">
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-    </row>
-    <row r="49" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="41" t="s">
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+    </row>
+    <row r="49" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="40" t="s">
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-    </row>
-    <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="41" t="s">
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+    </row>
+    <row r="50" spans="1:17" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="40" t="s">
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-    </row>
-    <row r="51" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+    </row>
+    <row r="51" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -3995,7 +3890,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -4004,7 +3899,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:17" s="33" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:17" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="35"/>
       <c r="B53" s="35"/>
       <c r="C53" s="35"/>
@@ -4023,7 +3918,7 @@
       <c r="P53" s="31"/>
       <c r="Q53" s="31"/>
     </row>
-    <row r="54" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -4032,7 +3927,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -4041,7 +3936,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -4050,7 +3945,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -4059,7 +3954,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -4068,7 +3963,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -4077,7 +3972,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -4086,7 +3981,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -4095,7 +3990,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -4104,7 +3999,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -4113,7 +4008,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="34" t="s">
         <v>48</v>
       </c>
@@ -4124,13 +4019,13 @@
       <c r="D64" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E64" s="57" t="s">
+      <c r="E64" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="57"/>
+      <c r="F64" s="53"/>
       <c r="G64" s="34"/>
     </row>
-    <row r="65" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="35" t="s">
         <v>46</v>
       </c>
@@ -4147,7 +4042,7 @@
       <c r="F65" s="35"/>
       <c r="G65" s="35"/>
     </row>
-    <row r="66" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="D66" s="29" t="s">
         <v>13</v>
       </c>
@@ -4157,7 +4052,7 @@
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
     </row>
-    <row r="67" spans="1:17" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="6"/>
@@ -4170,7 +4065,7 @@
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
     </row>
-    <row r="68" spans="1:17" s="33" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:17" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="35" t="s">
         <v>50</v>
       </c>
@@ -4193,6 +4088,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:C15"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:C23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:C31"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:C39"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="D50:G50"/>
@@ -4209,43 +4141,6 @@
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:G45"/>
     <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:C39"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:C31"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:C23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:C15"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
@@ -4254,10 +4149,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -4401,39 +4316,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4450,25 +4360,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>